<commit_message>
feat(app): added book importation
j'ai pu ajouter l'importation des livres ainsi que la Mainpage avec ces livres alignés avec un titre, résumé, date publication et aussi le nombre de pages.
Image couverture en WIP.
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_SallakuSamuel.xlsx
+++ b/doc/Journal-de-Travail_SallakuSamuel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pr13xpj\Documents\GitHub\P_MOBILE-PassionLecture-SamSallaku\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213A9723-AD7F-49CC-9717-23EC309C832A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32612865-16CC-497D-9386-FE8888505D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -187,6 +187,31 @@
   <si>
     <t>Il y a une erreur lorsqu'on clique sur le bouton "get books". Il n'arrive pas à récupérer les livres, en tout cas pas sur le  téléphone physique. A essayer sur l'émulateur</t>
   </si>
+  <si>
+    <t>J'ai cherché pour comment je puisse intéragir avec une API REST sur MAUI, et j'ai réussi à trouver une doc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Br_VfpKAbvI&amp;ab_channel=MacroCode</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/en-us/dotnet/maui/data-cloud/rest?view=net-maui-9.0</t>
+  </si>
+  <si>
+    <t>Après avoir lu la doc, j'ai pu mieux comprendre et j'ai donc implémenté cela dans mon app. J'ai eu des soucis où les données ne chargeaient pas, il me donnait une erreur à chaque fois étant: "[0:] The JSON value could not be converted to System.Collections.Generic.List1[P_PassionLecture.Models.Book]. Path: $ | LineNumber: 0 | BytePositionInLine: 1.: \tERROR {0}". J'ai donc cherché mais j'ai pas trouvé de méthode de convertir cela comme il faut.</t>
+  </si>
+  <si>
+    <t>J'ai rempli le JDT avec ce que j'ai fait aujourd'hui</t>
+  </si>
+  <si>
+    <t>J'ai donc demandé à chatgpt comment je pouvais améliorer cela, et il m'a dit de changer une ligne et ajouter cela: "                    var root = JsonDocument.Parse(content);
+                    var dataElement = root.RootElement.GetProperty("data");". J'ai cherché à comprendre ces lignes et donc ce que j'ai retenu est que la première ligne va prendre le JSON depuis le client et le rendre plus propre, afin qu'on puisse extraire les objets livres. Ensuite, la prochaine ligne va chercher les valeurs au début du tableau JSON que nous trouvions dans le backend, puis va le transformer dans une liste de livres que nous pourrions ajouter a la variable "books"</t>
+  </si>
+  <si>
+    <t>https://chatgpt.com/</t>
+  </si>
+  <si>
+    <t>J'ai fait des mises à jour dans le MainPage.xaml afin d'avoir des meilleurs résultats lors de l'importation des livres</t>
+  </si>
 </sst>
 </file>
 
@@ -200,7 +225,7 @@
     <numFmt numFmtId="168" formatCode="00\ &quot;min&quot;"/>
     <numFmt numFmtId="169" formatCode="hh\ &quot;h&quot;\ mm\ &quot;min&quot;"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -275,6 +300,14 @@
     <font>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -366,10 +399,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -505,8 +539,13 @@
     <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
@@ -1113,25 +1152,25 @@
                 <c:formatCode>hh\ "h"\ mm\ "min"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>6.9444444444444441E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.12847222222222221</c:v>
+                  <c:v>0.19097222222222221</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6.9444444444444441E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.10069444444444445</c:v>
+                  <c:v>0.1076388888888889</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.11458333333333333</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2.7777777777777776E-2</c:v>
@@ -2046,8 +2085,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2100,7 +2139,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 8 heurs 55 minutes</v>
+        <v>0 jours 11 heurs 10 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2115,15 +2154,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>415</v>
+        <v>490</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>535</v>
+        <v>670</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2584,75 +2623,131 @@
       <c r="G23" s="56"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="str">
+      <c r="A24" s="8">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="46"/>
+        <v>18</v>
+      </c>
+      <c r="B24" s="46">
+        <v>45779</v>
+      </c>
       <c r="C24" s="47"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="36"/>
+      <c r="D24" s="48">
+        <v>10</v>
+      </c>
+      <c r="E24" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>43</v>
+      </c>
       <c r="G24" s="55"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="str">
+    <row r="25" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="50"/>
+        <v>18</v>
+      </c>
+      <c r="B25" s="50">
+        <v>45779</v>
+      </c>
       <c r="C25" s="51"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="56"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="str">
+      <c r="D25" s="52">
+        <v>10</v>
+      </c>
+      <c r="E25" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" s="56" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v/>
-      </c>
-      <c r="B26" s="46"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="55"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="str">
+        <v>18</v>
+      </c>
+      <c r="B26" s="46">
+        <v>45779</v>
+      </c>
+      <c r="C26" s="47">
+        <v>1</v>
+      </c>
+      <c r="D26" s="48">
+        <v>10</v>
+      </c>
+      <c r="E26" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="59" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="16">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="50"/>
+        <v>18</v>
+      </c>
+      <c r="B27" s="50">
+        <v>45779</v>
+      </c>
       <c r="C27" s="51"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="56"/>
+      <c r="D27" s="52">
+        <v>20</v>
+      </c>
+      <c r="E27" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" s="56" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="str">
+      <c r="A28" s="8">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="46"/>
+        <v>18</v>
+      </c>
+      <c r="B28" s="46">
+        <v>45779</v>
+      </c>
       <c r="C28" s="47"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="35"/>
+      <c r="D28" s="48">
+        <v>15</v>
+      </c>
+      <c r="E28" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>55</v>
+      </c>
       <c r="G28" s="55"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="str">
+      <c r="A29" s="16">
         <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B29))</f>
-        <v/>
-      </c>
-      <c r="B29" s="50"/>
+        <v>18</v>
+      </c>
+      <c r="B29" s="50">
+        <v>45779</v>
+      </c>
       <c r="C29" s="51"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="35"/>
+      <c r="D29" s="52">
+        <v>10</v>
+      </c>
+      <c r="E29" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>52</v>
+      </c>
       <c r="G29" s="56"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -8734,10 +8829,13 @@
       <formula1>$M$7:$M$15</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G26" r:id="rId1" xr:uid="{096AEDFC-FEDE-4D4A-8ED1-086DDD047E45}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -8779,7 +8877,7 @@
       </c>
       <c r="B4">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C4,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C4" s="25" t="str">
         <f>'Journal de travail'!M8</f>
@@ -8787,17 +8885,17 @@
       </c>
       <c r="D4" s="33">
         <f>(A4+B4)/1440</f>
-        <v>0</v>
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>185</v>
+        <v>215</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8805,7 +8903,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.12847222222222221</v>
+        <v>0.19097222222222221</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8833,7 +8931,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C7" s="27" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8841,7 +8939,7 @@
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8851,7 +8949,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8859,7 +8957,7 @@
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
-        <v>0.10069444444444445</v>
+        <v>0.1076388888888889</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -8887,7 +8985,7 @@
       </c>
       <c r="B10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$D$7:$D$532)</f>
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="C10" s="37" t="str">
         <f>'Journal de travail'!M14</f>
@@ -8895,7 +8993,7 @@
       </c>
       <c r="D10" s="33">
         <f t="shared" si="0"/>
-        <v>0.11458333333333333</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -8922,7 +9020,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.37152777777777779</v>
+        <v>0.46527777777777779</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9159,6 +9257,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9167,15 +9274,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9198,6 +9296,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9206,12 +9312,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(app): added detailpage + fix mainpage
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_SallakuSamuel.xlsx
+++ b/doc/Journal-de-Travail_SallakuSamuel.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pr13xpj\Documents\GitHub\P_MOBILE-PassionLecture-SamSallaku\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32612865-16CC-497D-9386-FE8888505D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DC43C2-0B8E-4D40-A54C-7D73BB94961F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -211,6 +211,24 @@
   </si>
   <si>
     <t>J'ai fait des mises à jour dans le MainPage.xaml afin d'avoir des meilleurs résultats lors de l'importation des livres</t>
+  </si>
+  <si>
+    <t>Meeting avec le prof</t>
+  </si>
+  <si>
+    <t>J'ai dû trouver un moyen de récupérer les données du backend sur le téléphone physique car il marchait seulement sur l'émulateur, et j'ai trouvé ngrok</t>
+  </si>
+  <si>
+    <t>https://dashboard.ngrok.com/get-started/setup/windows</t>
+  </si>
+  <si>
+    <t>J'ai continué sur les livres, il fallait que je fasse un autre alignement car c'était très lent et on pourrait afficher que 4 livres à la fois. J'ai donc changé le xaml</t>
+  </si>
+  <si>
+    <t>JDT</t>
+  </si>
+  <si>
+    <t>J'ai commencé à faire la page de détail d'un livre</t>
   </si>
 </sst>
 </file>
@@ -532,16 +550,16 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1155,16 +1173,16 @@
                   <c:v>6.9444444444444441E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19097222222222221</c:v>
+                  <c:v>0.2673611111111111</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.9444444444444441E-3</c:v>
+                  <c:v>1.0416666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1076388888888889</c:v>
+                  <c:v>0.12152777777777778</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2085,8 +2103,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+      <pane ySplit="6" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2121,11 +2139,11 @@
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2139,7 +2157,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 11 heurs 10 minutes</v>
+        <v>0 jours 13 heurs 25 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2154,24 +2172,24 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>490</v>
+        <v>565</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>670</v>
+        <v>805</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="58"/>
+      <c r="D5" s="59"/>
     </row>
     <row r="6" spans="1:15" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
@@ -2684,7 +2702,7 @@
       <c r="F26" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="G26" s="59" t="s">
+      <c r="G26" s="57" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2751,63 +2769,105 @@
       <c r="G29" s="56"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="str">
+      <c r="A30" s="8">
         <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B30))</f>
-        <v/>
-      </c>
-      <c r="B30" s="46"/>
+        <v>19</v>
+      </c>
+      <c r="B30" s="46">
+        <v>45786</v>
+      </c>
       <c r="C30" s="47"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="36"/>
+      <c r="D30" s="48">
+        <v>20</v>
+      </c>
+      <c r="E30" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="36" t="s">
+        <v>56</v>
+      </c>
       <c r="G30" s="55"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="str">
+      <c r="A31" s="16">
         <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B31))</f>
-        <v/>
-      </c>
-      <c r="B31" s="50"/>
+        <v>19</v>
+      </c>
+      <c r="B31" s="50">
+        <v>45786</v>
+      </c>
       <c r="C31" s="51"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="56"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="str">
+      <c r="D31" s="52">
+        <v>40</v>
+      </c>
+      <c r="E31" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" s="56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
         <f>IF(ISBLANK(B32),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B32))</f>
-        <v/>
-      </c>
-      <c r="B32" s="46"/>
-      <c r="C32" s="47"/>
+        <v>19</v>
+      </c>
+      <c r="B32" s="46">
+        <v>45786</v>
+      </c>
+      <c r="C32" s="47">
+        <v>1</v>
+      </c>
       <c r="D32" s="48"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="36"/>
+      <c r="E32" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="36" t="s">
+        <v>59</v>
+      </c>
       <c r="G32" s="55"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="str">
+      <c r="A33" s="16">
         <f>IF(ISBLANK(B33),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B33))</f>
-        <v/>
-      </c>
-      <c r="B33" s="50"/>
+        <v>19</v>
+      </c>
+      <c r="B33" s="50">
+        <v>45786</v>
+      </c>
       <c r="C33" s="51"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="35"/>
+      <c r="D33" s="52">
+        <v>10</v>
+      </c>
+      <c r="E33" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>61</v>
+      </c>
       <c r="G33" s="56"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="str">
+      <c r="A34" s="8">
         <f>IF(ISBLANK(B34),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B34))</f>
-        <v/>
-      </c>
-      <c r="B34" s="46"/>
+        <v>19</v>
+      </c>
+      <c r="B34" s="46">
+        <v>45786</v>
+      </c>
       <c r="C34" s="47"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="49"/>
-      <c r="F34" s="35"/>
+      <c r="D34" s="48">
+        <v>5</v>
+      </c>
+      <c r="E34" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>60</v>
+      </c>
       <c r="G34" s="55"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -8891,11 +8951,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>215</v>
+        <v>265</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8903,7 +8963,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.19097222222222221</v>
+        <v>0.2673611111111111</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8931,7 +8991,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C7" s="27" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8939,7 +8999,7 @@
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
-        <v>6.9444444444444441E-3</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8949,7 +9009,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8957,7 +9017,7 @@
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
-        <v>0.1076388888888889</v>
+        <v>0.12152777777777778</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -9020,7 +9080,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.46527777777777779</v>
+        <v>0.55902777777777779</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9257,15 +9317,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9274,6 +9325,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9296,14 +9356,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9312,4 +9364,12 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(app): fully functional app
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_SallakuSamuel.xlsx
+++ b/doc/Journal-de-Travail_SallakuSamuel.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pr13xpj\Documents\GitHub\P_MOBILE-PassionLecture-SamSallaku\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Documents\GitHub\P_MOBILE-PassionLecture-SamSallaku\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E186BDFB-A3B6-4200-B85A-31699C56C6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0D4F50-27E8-4BCD-A282-8E57988573BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="1440" yWindow="825" windowWidth="26415" windowHeight="13725" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -244,6 +244,24 @@
   </si>
   <si>
     <t>J'ai essayé de faire les tags en utilisant la DB locale, donc SQLite mais jai eu une exception et après des recherches j'ai dû faire un "Batteries.Init" dans le MauiProgram.cs. Même après ça, ca ne marchait pas</t>
+  </si>
+  <si>
+    <t>J'ai essayé de faire l'importation des EPUB mais cela n'a pas fonctionné. J'ai aussi essayé d'adapter le backend pour cela, donc faire une route qui prend les epu/blob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting avec le prof pour l'évaluation </t>
+  </si>
+  <si>
+    <t>J'ai réussi à faire fonctionner le backend mais je n'arrive pas à les lire sur l'app, il me retourne une erreur 404 à chaque fois</t>
+  </si>
+  <si>
+    <t>J'ai réussi à lire les epubs et l'erreur était en effet dans le backend car ma route était mal nommée quand je l'ai appelé sur le code</t>
+  </si>
+  <si>
+    <t>J'ai reglé le format, car quand on lisait les livres il y avait des balises HTML en trop</t>
+  </si>
+  <si>
+    <t>J'ai continué sur la page de recherche, j'ai pu faire en sorte que les tags s'affichent ainsi que la recherche par tag, date de publication et titre de livre.</t>
   </si>
 </sst>
 </file>
@@ -578,10 +596,84 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -754,80 +846,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -850,7 +868,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -917,7 +935,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1188,16 +1206,16 @@
                   <c:v>6.9444444444444441E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32291666666666669</c:v>
+                  <c:v>0.51041666666666663</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7777777777777776E-2</c:v>
+                  <c:v>3.8194444444444448E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1388888888888889</c:v>
+                  <c:v>0.14583333333333334</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1912,18 +1930,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2118,11 +2136,11 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F38" sqref="F38"/>
+      <pane ySplit="6" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.625" style="8" customWidth="1"/>
     <col min="2" max="2" width="10.625" style="1" customWidth="1"/>
@@ -2172,7 +2190,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 15 heurs 35 minutes</v>
+        <v>0 jours 20 heurs 30 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2187,15 +2205,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>695</v>
+        <v>870</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>935</v>
+        <v>1230</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2947,7 +2965,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <f>IF(ISBLANK(B38),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B38))</f>
         <v>20</v>
@@ -2990,99 +3008,165 @@
       <c r="G39" s="56"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="str">
+      <c r="A40" s="8">
         <f>IF(ISBLANK(B40),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B40))</f>
-        <v/>
-      </c>
-      <c r="B40" s="46"/>
+        <v>21</v>
+      </c>
+      <c r="B40" s="46">
+        <v>45800</v>
+      </c>
       <c r="C40" s="47"/>
-      <c r="D40" s="48"/>
-      <c r="E40" s="49"/>
-      <c r="F40" s="35"/>
+      <c r="D40" s="48">
+        <v>50</v>
+      </c>
+      <c r="E40" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="35" t="s">
+        <v>67</v>
+      </c>
       <c r="G40" s="55"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="str">
+      <c r="A41" s="16">
         <f>IF(ISBLANK(B41),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B41))</f>
-        <v/>
-      </c>
-      <c r="B41" s="50"/>
+        <v>21</v>
+      </c>
+      <c r="B41" s="50">
+        <v>45800</v>
+      </c>
       <c r="C41" s="51"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="35"/>
+      <c r="D41" s="52">
+        <v>10</v>
+      </c>
+      <c r="E41" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>68</v>
+      </c>
       <c r="G41" s="56"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="str">
+      <c r="A42" s="8">
         <f>IF(ISBLANK(B42),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B42))</f>
-        <v/>
-      </c>
-      <c r="B42" s="46"/>
-      <c r="C42" s="47"/>
+        <v>21</v>
+      </c>
+      <c r="B42" s="46">
+        <v>45800</v>
+      </c>
+      <c r="C42" s="47">
+        <v>1</v>
+      </c>
       <c r="D42" s="48"/>
-      <c r="E42" s="49"/>
-      <c r="F42" s="35"/>
+      <c r="E42" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="35" t="s">
+        <v>69</v>
+      </c>
       <c r="G42" s="55"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="str">
+      <c r="A43" s="16">
         <f>IF(ISBLANK(B43),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B43))</f>
-        <v/>
-      </c>
-      <c r="B43" s="50"/>
+        <v>21</v>
+      </c>
+      <c r="B43" s="50">
+        <v>45800</v>
+      </c>
       <c r="C43" s="51"/>
-      <c r="D43" s="52"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="35"/>
+      <c r="D43" s="52">
+        <v>10</v>
+      </c>
+      <c r="E43" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" s="35" t="s">
+        <v>60</v>
+      </c>
       <c r="G43" s="56"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="str">
+      <c r="A44" s="8">
         <f>IF(ISBLANK(B44),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B44))</f>
-        <v/>
-      </c>
-      <c r="B44" s="46"/>
+        <v>22</v>
+      </c>
+      <c r="B44" s="46">
+        <v>45804</v>
+      </c>
       <c r="C44" s="47"/>
-      <c r="D44" s="48"/>
-      <c r="E44" s="49"/>
-      <c r="F44" s="35"/>
+      <c r="D44" s="48">
+        <v>40</v>
+      </c>
+      <c r="E44" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="35" t="s">
+        <v>70</v>
+      </c>
       <c r="G44" s="55"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="str">
+      <c r="A45" s="16">
         <f>IF(ISBLANK(B45),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B45))</f>
-        <v/>
-      </c>
-      <c r="B45" s="50"/>
+        <v>22</v>
+      </c>
+      <c r="B45" s="50">
+        <v>45804</v>
+      </c>
       <c r="C45" s="51"/>
-      <c r="D45" s="52"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="35"/>
+      <c r="D45" s="52">
+        <v>30</v>
+      </c>
+      <c r="E45" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" s="35" t="s">
+        <v>71</v>
+      </c>
       <c r="G45" s="56"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="str">
+      <c r="A46" s="8">
         <f>IF(ISBLANK(B46),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B46))</f>
-        <v/>
-      </c>
-      <c r="B46" s="46"/>
-      <c r="C46" s="47"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="35"/>
+        <v>22</v>
+      </c>
+      <c r="B46" s="46">
+        <v>45805</v>
+      </c>
+      <c r="C46" s="47">
+        <v>1</v>
+      </c>
+      <c r="D46" s="48">
+        <v>30</v>
+      </c>
+      <c r="E46" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" s="35" t="s">
+        <v>72</v>
+      </c>
       <c r="G46" s="55"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="str">
+      <c r="A47" s="16">
         <f>IF(ISBLANK(B47),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B47))</f>
-        <v/>
-      </c>
-      <c r="B47" s="50"/>
+        <v>22</v>
+      </c>
+      <c r="B47" s="50">
+        <v>45805</v>
+      </c>
       <c r="C47" s="51"/>
-      <c r="D47" s="52"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="35"/>
+      <c r="D47" s="52">
+        <v>5</v>
+      </c>
+      <c r="E47" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" s="35" t="s">
+        <v>60</v>
+      </c>
       <c r="G47" s="56"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -8912,28 +8996,28 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E532">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8968,7 +9052,7 @@
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="10.875" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="29" bestFit="1" customWidth="1"/>
@@ -9010,11 +9094,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>345</v>
+        <v>495</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -9022,7 +9106,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.32291666666666669</v>
+        <v>0.51041666666666663</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -9050,7 +9134,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C7" s="27" t="str">
         <f>'Journal de travail'!M11</f>
@@ -9058,7 +9142,7 @@
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
-        <v>2.7777777777777776E-2</v>
+        <v>3.8194444444444448E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -9068,7 +9152,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>'Journal de travail'!M12</f>
@@ -9076,7 +9160,7 @@
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
-        <v>0.1388888888888889</v>
+        <v>0.14583333333333334</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -9139,7 +9223,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.64930555555555558</v>
+        <v>0.85416666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9153,6 +9237,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9375,27 +9479,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9412,23 +9515,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>